<commit_message>
Modeling The Plasma Emitter in Navy Paper
Modeling The Plasma Emitter in Navy Paper
</commit_message>
<xml_diff>
--- a/Investments-In-Alternative-Fusion-December-2014.xlsx
+++ b/Investments-In-Alternative-Fusion-December-2014.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthew\Documents\GitHub\Polywell-Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -664,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -818,6 +818,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1111,8 +1112,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:AH132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1127,22 +1128,22 @@
     <col min="10" max="11" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="68" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="68" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="68" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -1153,7 +1154,7 @@
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="54" t="s">
         <v>117</v>
@@ -1180,7 +1181,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="15"/>
       <c r="B9" s="7" t="s">
         <v>112</v>
@@ -1205,7 +1206,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
       <c r="B10" s="19" t="s">
         <v>113</v>
@@ -1230,7 +1231,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="15"/>
       <c r="B11" s="7" t="s">
         <v>113</v>
@@ -1257,7 +1258,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="15"/>
       <c r="B12" s="19" t="s">
         <v>114</v>
@@ -1284,7 +1285,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="19" t="s">
         <v>114</v>
@@ -1311,7 +1312,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="19" t="s">
         <v>114</v>
@@ -1338,7 +1339,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="19" t="s">
         <v>114</v>
@@ -1365,7 +1366,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="9" t="s">
         <v>115</v>
@@ -1391,8 +1392,12 @@
       <c r="I16" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K16" s="69">
+        <f>SUM(D12:D15)</f>
+        <v>4480279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="9" t="s">
         <v>115</v>
@@ -1419,7 +1424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="20" t="s">
         <v>115</v>
@@ -1446,7 +1451,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="B19" s="20" t="s">
         <v>115</v>
@@ -1473,7 +1478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="15"/>
       <c r="B20" s="20" t="s">
         <v>115</v>
@@ -1500,7 +1505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="15"/>
       <c r="B21" s="20" t="s">
         <v>115</v>
@@ -1527,7 +1532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="20" t="s">
         <v>115</v>
@@ -1553,8 +1558,12 @@
       <c r="I22" s="27" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K22" s="69">
+        <f>SUM(D16:D25)+SUM(D27:D30)</f>
+        <v>151500000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
       <c r="B23" s="20" t="s">
         <v>115</v>
@@ -1581,7 +1590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="20" t="s">
         <v>115</v>
@@ -1608,7 +1617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="B25" s="20" t="s">
         <v>115</v>
@@ -1636,7 +1645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="9" t="s">
         <v>112</v>
@@ -1663,7 +1672,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="20" t="s">
         <v>115</v>
@@ -1690,7 +1699,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="20" t="s">
         <v>115</v>
@@ -1717,7 +1726,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="20" t="s">
         <v>115</v>
@@ -1745,7 +1754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="15"/>
       <c r="B30" s="20" t="s">
         <v>115</v>
@@ -1772,7 +1781,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="20" t="s">
         <v>115</v>
@@ -1799,7 +1808,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="9" t="s">
         <v>116</v>
@@ -3448,6 +3457,7 @@
     </row>
     <row r="95" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A95" s="6"/>
+      <c r="D95" s="69"/>
       <c r="F95" s="6"/>
       <c r="H95" s="6"/>
       <c r="I95" s="6"/>

</xml_diff>